<commit_message>
added 4 yield contracts
</commit_message>
<xml_diff>
--- a/element.xlsx
+++ b/element.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clickdee\element\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF15AED2-81A0-497D-A31D-3BB0EDCFBD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAFE087-7041-4B39-8EE4-53BBF32D8EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A9B8B1C-1B5C-49F6-83F4-46CC389FFD50}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
   <si>
     <t>Liquidity pool contract Addresses</t>
   </si>
@@ -208,13 +208,207 @@
   <si>
     <t>alUSD3CRV-f - ePyvCurve-alUSD
 Jan 28, 2022</t>
+  </si>
+  <si>
+    <t>yield contract addresses</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>0x415747EE98D482e6dD9B431fa76Ad5553744F247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+DAI - eYyvDAI
+ Apr 30, 2022</t>
+  </si>
+  <si>
+    <t>0x8E9d636BbE6939BD0F52849afc02C0c66F6A3603</t>
+  </si>
+  <si>
+    <t>LUSD3CRV-f - eYyvCurveLUSD
+ Apr 30, 2022</t>
+  </si>
+  <si>
+    <t>0xCF354603A9AEbD2Ff9f33E1B04246d8Ea204ae95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+WBTC - eYyvWBTC
+ Apr 30, 2022</t>
+  </si>
+  <si>
+    <t>0x7173b184525feAD2fFbde5FBe6FCB65Ea8246eE7</t>
+  </si>
+  <si>
+    <t>USDC - eYyvUSDC
+ Apr 29, 2022</t>
+  </si>
+  <si>
+    <t>0x4aBB6FD289fA70056CFcB58ceBab8689921eB922</t>
+  </si>
+  <si>
+    <t>crv3crypto - eYyvcrv3crypto
+Apr 29, 2022</t>
+  </si>
+  <si>
+    <t>0x7C9cF12d783821d5C63d8E9427aF5C44bAd92445</t>
+  </si>
+  <si>
+    <t>USDC - eYyvUSDC
+Dec 17, 2021</t>
+  </si>
+  <si>
+    <t>0x062F38735AAC32320DB5e2DBBEb07968351D7C72</t>
+  </si>
+  <si>
+    <t>steCRV - eYyvcrvSTETH
+ Apr 15, 2022</t>
+  </si>
+  <si>
+    <t>0xB70c25D96EF260eA07F650037Bf68F5d6583885e</t>
+  </si>
+  <si>
+    <t>DAI - eYyvDAI
+Jan 28, 2022</t>
+  </si>
+  <si>
+    <t>0x4212bE3C7b255bA4B29705573ABD023cdcE21542</t>
+  </si>
+  <si>
+    <t>steCRV - eYyvcrvSTETH
+Jan 28, 2022</t>
+  </si>
+  <si>
+    <t>0x9e030b67a8384cbba09D5927533Aa98010C87d91</t>
+  </si>
+  <si>
+    <t>USDC - eYyvUSDC
+ Jan 28, 2022</t>
+  </si>
+  <si>
+    <t>0x7320d680Ca9BCE8048a286f00A79A2c9f8DCD7b3</t>
+  </si>
+  <si>
+    <t>WBTC - eYyvWBTC
+Nov 26, 2021</t>
+  </si>
+  <si>
+    <t>0xd16847480D6bc218048CD31Ad98b63CC34e5c2bF</t>
+  </si>
+  <si>
+    <t>crv3crypto - eYyvcrv3crypto
+Nov 13, 2021</t>
+  </si>
+  <si>
+    <t>0x2D6e3515C8b47192Ca3913770fa741d3C4Dac354</t>
+  </si>
+  <si>
+    <t>USDC - eYyvUSDC
+Oct 29, 2021</t>
+  </si>
+  <si>
+    <t>0xE54B3F5c444a801e61BECDCa93e74CdC1C4C1F90</t>
+  </si>
+  <si>
+    <t>DAI - eYyvDAI
+ Oct 16, 2021</t>
+  </si>
+  <si>
+    <t>0xD5D7bc115B32ad1449C6D0083E43C87be95F2809</t>
+  </si>
+  <si>
+    <t>steCRV - eYyvcrvSTETH
+Oct 16, 2021</t>
+  </si>
+  <si>
+    <t>0xF94A7Df264A2ec8bCEef2cFE54d7cA3f6C6DFC7a</t>
+  </si>
+  <si>
+    <t>crvTricrypto - eYyvCrvTriCrypto
+Aug 15, 2021</t>
+  </si>
+  <si>
+    <t>0x67F8FCb9D3c463da05DE1392EfDbB2A87F8599Ea</t>
+  </si>
+  <si>
+    <t>LUSD3CRV-f - eYyvCurveLUSD
+Dec 27, 2021</t>
+  </si>
+  <si>
+    <t>0xDe620bb8BE43ee54d7aa73f8E99A7409Fe511084</t>
+  </si>
+  <si>
+    <t>LUSD3CRV-f - eYyvCurveLUSD
+Sep 28, 2021</t>
+  </si>
+  <si>
+    <t>alUSD3CRV-f - ePyvCurve-alUSD
+ Apr 30, 2022</t>
+  </si>
+  <si>
+    <t>0x6FE95FafE2F86158c77Bf18350672D360BfC78a2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MIM-3LP3CRV-f - eYyvCurve-MIM
+ Apr 29, 2022</t>
+  </si>
+  <si>
+    <t>0x5fA3ce1fB47bC8A29B5C02e2e7167799BBAf5F41</t>
+  </si>
+  <si>
+    <t>eursCRV - eYyvCurve-EURS
+ Feb 12, 2022</t>
+  </si>
+  <si>
+    <t>0x1D310a6238e11c8BE91D83193C88A99eB66279bE</t>
+  </si>
+  <si>
+    <t>MIM-3LP3CRV-f - eYyvCurve-MIM
+Feb 11, 2022</t>
+  </si>
+  <si>
+    <t>0x802d0f2f4b5f1fb5BfC9b2040a703c1464e1D4CB</t>
+  </si>
+  <si>
+    <t>alUSD3CRV-f - eYyvCurve-alUSD
+Jan 28, 2022</t>
+  </si>
+  <si>
+    <t>Yield contract address</t>
+  </si>
+  <si>
+    <t>0xCFe60a1535ecc5B0bc628dC97111C8bb01637911</t>
+  </si>
+  <si>
+    <t>USDC-sep17-2022</t>
+  </si>
+  <si>
+    <t>0x52C9886d5D87B0f06EbACBEff750B5Ffad5d17d9</t>
+  </si>
+  <si>
+    <t>USDC-apr29-2022</t>
+  </si>
+  <si>
+    <t>0x2c72692E94E757679289aC85d3556b2c0f717E0E</t>
+  </si>
+  <si>
+    <t>DAI-apr30-2022</t>
+  </si>
+  <si>
+    <t>0x49e9e169f0B661Ea0A883f490564F4CC275123Ed</t>
+  </si>
+  <si>
+    <t>WBTC-apr30-2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +429,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -261,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -274,6 +476,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6086B0-CA5C-41CB-A5C0-EF3C564A5FF6}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,10 +808,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -799,6 +1005,238 @@
       </c>
       <c r="B27" s="3" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>